<commit_message>
dynamic data for chart
</commit_message>
<xml_diff>
--- a/import_request.xlsx
+++ b/import_request.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Part</t>
   </si>
@@ -23,18 +23,6 @@
   </si>
   <si>
     <t>Money</t>
-  </si>
-  <si>
-    <t>5mm</t>
-  </si>
-  <si>
-    <t>ka001</t>
-  </si>
-  <si>
-    <t>kh001</t>
-  </si>
-  <si>
-    <t>KV120</t>
   </si>
 </sst>
 </file>
@@ -411,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="10" customWidth="1"/>
@@ -432,62 +420,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4">
-        <v>31</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>2</v>
-      </c>
-      <c r="D5">
-        <v>40</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>